<commit_message>
D0 W data added
</commit_message>
<xml_diff>
--- a/dy_qT/expdata/90006.xlsx
+++ b/dy_qT/expdata/90006.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/avp5627/GIT/database/dy_qT/expdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FD3C24E-D4D2-DC4F-A32A-EC186E252B96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60E9DE96-D04C-6044-99D0-85A14D31EB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7080" yWindow="1720" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CDF1" sheetId="1" r:id="rId1"/>
@@ -950,8 +950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:K21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1035,13 +1035,13 @@
         <v>1800</v>
       </c>
       <c r="B2">
-        <v>91</v>
-      </c>
-      <c r="C2">
-        <v>66</v>
-      </c>
-      <c r="D2">
-        <v>116</v>
+        <v>80.379000000000005</v>
+      </c>
+      <c r="C2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D2" t="b">
+        <v>0</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -1106,13 +1106,13 @@
         <v>1800</v>
       </c>
       <c r="B3">
-        <v>91</v>
-      </c>
-      <c r="C3">
-        <v>66</v>
-      </c>
-      <c r="D3">
-        <v>116</v>
+        <v>80.379000000000005</v>
+      </c>
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" t="b">
+        <v>0</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -1177,13 +1177,13 @@
         <v>1800</v>
       </c>
       <c r="B4">
-        <v>91</v>
-      </c>
-      <c r="C4">
-        <v>66</v>
-      </c>
-      <c r="D4">
-        <v>116</v>
+        <v>80.379000000000005</v>
+      </c>
+      <c r="C4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" t="b">
+        <v>0</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -1248,13 +1248,13 @@
         <v>1800</v>
       </c>
       <c r="B5">
-        <v>91</v>
-      </c>
-      <c r="C5">
-        <v>66</v>
-      </c>
-      <c r="D5">
-        <v>116</v>
+        <v>80.379000000000005</v>
+      </c>
+      <c r="C5" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" t="b">
+        <v>0</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -1319,13 +1319,13 @@
         <v>1800</v>
       </c>
       <c r="B6">
-        <v>91</v>
-      </c>
-      <c r="C6">
-        <v>66</v>
-      </c>
-      <c r="D6">
-        <v>116</v>
+        <v>80.379000000000005</v>
+      </c>
+      <c r="C6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" t="b">
+        <v>0</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -1390,13 +1390,13 @@
         <v>1800</v>
       </c>
       <c r="B7">
-        <v>91</v>
-      </c>
-      <c r="C7">
-        <v>66</v>
-      </c>
-      <c r="D7">
-        <v>116</v>
+        <v>80.379000000000005</v>
+      </c>
+      <c r="C7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" t="b">
+        <v>0</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -1461,13 +1461,13 @@
         <v>1800</v>
       </c>
       <c r="B8">
-        <v>91</v>
-      </c>
-      <c r="C8">
-        <v>66</v>
-      </c>
-      <c r="D8">
-        <v>116</v>
+        <v>80.379000000000005</v>
+      </c>
+      <c r="C8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" t="b">
+        <v>0</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -1532,13 +1532,13 @@
         <v>1800</v>
       </c>
       <c r="B9">
-        <v>91</v>
-      </c>
-      <c r="C9">
-        <v>66</v>
-      </c>
-      <c r="D9">
-        <v>116</v>
+        <v>80.379000000000005</v>
+      </c>
+      <c r="C9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D9" t="b">
+        <v>0</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -1603,13 +1603,13 @@
         <v>1800</v>
       </c>
       <c r="B10">
-        <v>91</v>
-      </c>
-      <c r="C10">
-        <v>66</v>
-      </c>
-      <c r="D10">
-        <v>116</v>
+        <v>80.379000000000005</v>
+      </c>
+      <c r="C10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10" t="b">
+        <v>0</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -1674,13 +1674,13 @@
         <v>1800</v>
       </c>
       <c r="B11">
-        <v>91</v>
-      </c>
-      <c r="C11">
-        <v>66</v>
-      </c>
-      <c r="D11">
-        <v>116</v>
+        <v>80.379000000000005</v>
+      </c>
+      <c r="C11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D11" t="b">
+        <v>0</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -1745,13 +1745,13 @@
         <v>1800</v>
       </c>
       <c r="B12">
-        <v>91</v>
-      </c>
-      <c r="C12">
-        <v>66</v>
-      </c>
-      <c r="D12">
-        <v>116</v>
+        <v>80.379000000000005</v>
+      </c>
+      <c r="C12" t="b">
+        <v>0</v>
+      </c>
+      <c r="D12" t="b">
+        <v>0</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -1816,13 +1816,13 @@
         <v>1800</v>
       </c>
       <c r="B13">
-        <v>91</v>
-      </c>
-      <c r="C13">
-        <v>66</v>
-      </c>
-      <c r="D13">
-        <v>116</v>
+        <v>80.379000000000005</v>
+      </c>
+      <c r="C13" t="b">
+        <v>0</v>
+      </c>
+      <c r="D13" t="b">
+        <v>0</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -1887,13 +1887,13 @@
         <v>1800</v>
       </c>
       <c r="B14">
-        <v>91</v>
-      </c>
-      <c r="C14">
-        <v>66</v>
-      </c>
-      <c r="D14">
-        <v>116</v>
+        <v>80.379000000000005</v>
+      </c>
+      <c r="C14" t="b">
+        <v>0</v>
+      </c>
+      <c r="D14" t="b">
+        <v>0</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -1958,13 +1958,13 @@
         <v>1800</v>
       </c>
       <c r="B15">
-        <v>91</v>
-      </c>
-      <c r="C15">
-        <v>66</v>
-      </c>
-      <c r="D15">
-        <v>116</v>
+        <v>80.379000000000005</v>
+      </c>
+      <c r="C15" t="b">
+        <v>0</v>
+      </c>
+      <c r="D15" t="b">
+        <v>0</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -2029,13 +2029,13 @@
         <v>1800</v>
       </c>
       <c r="B16">
-        <v>91</v>
-      </c>
-      <c r="C16">
-        <v>66</v>
-      </c>
-      <c r="D16">
-        <v>116</v>
+        <v>80.379000000000005</v>
+      </c>
+      <c r="C16" t="b">
+        <v>0</v>
+      </c>
+      <c r="D16" t="b">
+        <v>0</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -2100,13 +2100,13 @@
         <v>1800</v>
       </c>
       <c r="B17">
-        <v>91</v>
-      </c>
-      <c r="C17">
-        <v>66</v>
-      </c>
-      <c r="D17">
-        <v>116</v>
+        <v>80.379000000000005</v>
+      </c>
+      <c r="C17" t="b">
+        <v>0</v>
+      </c>
+      <c r="D17" t="b">
+        <v>0</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -2171,13 +2171,13 @@
         <v>1800</v>
       </c>
       <c r="B18">
-        <v>91</v>
-      </c>
-      <c r="C18">
-        <v>66</v>
-      </c>
-      <c r="D18">
-        <v>116</v>
+        <v>80.379000000000005</v>
+      </c>
+      <c r="C18" t="b">
+        <v>0</v>
+      </c>
+      <c r="D18" t="b">
+        <v>0</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -2242,13 +2242,13 @@
         <v>1800</v>
       </c>
       <c r="B19">
-        <v>91</v>
-      </c>
-      <c r="C19">
-        <v>66</v>
-      </c>
-      <c r="D19">
-        <v>116</v>
+        <v>80.379000000000005</v>
+      </c>
+      <c r="C19" t="b">
+        <v>0</v>
+      </c>
+      <c r="D19" t="b">
+        <v>0</v>
       </c>
       <c r="E19">
         <v>0</v>
@@ -2313,13 +2313,13 @@
         <v>1800</v>
       </c>
       <c r="B20">
-        <v>91</v>
-      </c>
-      <c r="C20">
-        <v>66</v>
-      </c>
-      <c r="D20">
-        <v>116</v>
+        <v>80.379000000000005</v>
+      </c>
+      <c r="C20" t="b">
+        <v>0</v>
+      </c>
+      <c r="D20" t="b">
+        <v>0</v>
       </c>
       <c r="E20">
         <v>0</v>
@@ -2384,13 +2384,13 @@
         <v>1800</v>
       </c>
       <c r="B21">
-        <v>91</v>
-      </c>
-      <c r="C21">
-        <v>66</v>
-      </c>
-      <c r="D21">
-        <v>116</v>
+        <v>80.379000000000005</v>
+      </c>
+      <c r="C21" t="b">
+        <v>0</v>
+      </c>
+      <c r="D21" t="b">
+        <v>0</v>
       </c>
       <c r="E21">
         <v>0</v>

</xml_diff>